<commit_message>
Kate is updating script and data
</commit_message>
<xml_diff>
--- a/Data/NE_Pipe_and_Samples.xlsx
+++ b/Data/NE_Pipe_and_Samples.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kateg\Diss_2022\Pb_Diss_KM\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D82F78E-CF14-4BD6-ACFB-0857FECDB0DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70F64036-526A-4779-A865-98495ABC0C6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{6660F883-04A9-4EBD-9AC1-2C8B779AA34C}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="NE_Pipe_and_Samples" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="50">
   <si>
     <t>IV305GP</t>
   </si>
@@ -158,9 +157,6 @@
     <t>UK coal</t>
   </si>
   <si>
-    <t>Geological</t>
-  </si>
-  <si>
     <t>UK petrol</t>
   </si>
   <si>
@@ -173,7 +169,22 @@
     <t>St_dev_y</t>
   </si>
   <si>
-    <t>Water sample</t>
+    <t>Edi/EL pipe</t>
+  </si>
+  <si>
+    <t>G pipe</t>
+  </si>
+  <si>
+    <t>NJ Water sample</t>
+  </si>
+  <si>
+    <t>Geological (river)</t>
+  </si>
+  <si>
+    <t>Geological (lake)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Geological (peat) </t>
   </si>
 </sst>
 </file>
@@ -192,12 +203,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -212,12 +229,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -251,7 +269,17 @@
   <c:chart>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.1190545089020539E-2"/>
+          <c:y val="4.9971598103869384E-2"/>
+          <c:w val="0.70987536615950086"/>
+          <c:h val="0.86735599094000981"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -260,7 +288,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>NE_Pipe_and_Samples!$B$2</c:f>
+              <c:f>NE_Pipe_and_Samples!$B$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -298,7 +326,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>NE_Pipe_and_Samples!$H$2</c:f>
+                <c:f>NE_Pipe_and_Samples!$H$4</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="1"/>
@@ -310,7 +338,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>NE_Pipe_and_Samples!$H$2</c:f>
+                <c:f>NE_Pipe_and_Samples!$H$4</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="1"/>
@@ -341,7 +369,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>NE_Pipe_and_Samples!$J$2</c:f>
+                <c:f>NE_Pipe_and_Samples!$J$4</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="1"/>
@@ -353,7 +381,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>NE_Pipe_and_Samples!$J$2</c:f>
+                <c:f>NE_Pipe_and_Samples!$J$4</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="1"/>
@@ -379,24 +407,24 @@
           </c:errBars>
           <c:xVal>
             <c:numRef>
-              <c:f>NE_Pipe_and_Samples!$G$2</c:f>
+              <c:f>NE_Pipe_and_Samples!$G$4</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1.1326363249560998</c:v>
+                  <c:v>1.133</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>NE_Pipe_and_Samples!$I$2</c:f>
+              <c:f>NE_Pipe_and_Samples!$I$4</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2.4255835968166899</c:v>
+                  <c:v>2.4355835968166897</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -413,7 +441,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>NE_Pipe_and_Samples!$B$3</c:f>
+              <c:f>NE_Pipe_and_Samples!$B$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -451,7 +479,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>NE_Pipe_and_Samples!$H$3</c:f>
+                <c:f>NE_Pipe_and_Samples!$H$5</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="1"/>
@@ -463,7 +491,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>NE_Pipe_and_Samples!$H$3</c:f>
+                <c:f>NE_Pipe_and_Samples!$H$5</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="1"/>
@@ -494,7 +522,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>NE_Pipe_and_Samples!$J$3</c:f>
+                <c:f>NE_Pipe_and_Samples!$J$5</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="1"/>
@@ -506,7 +534,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>NE_Pipe_and_Samples!$J$3</c:f>
+                <c:f>NE_Pipe_and_Samples!$J$5</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="1"/>
@@ -532,7 +560,7 @@
           </c:errBars>
           <c:xVal>
             <c:numRef>
-              <c:f>NE_Pipe_and_Samples!$G$3</c:f>
+              <c:f>NE_Pipe_and_Samples!$G$5</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="1"/>
@@ -544,7 +572,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>NE_Pipe_and_Samples!$I$3</c:f>
+              <c:f>NE_Pipe_and_Samples!$I$5</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="1"/>
@@ -566,7 +594,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>NE_Pipe_and_Samples!$B$4</c:f>
+              <c:f>NE_Pipe_and_Samples!$B$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -592,312 +620,6 @@
               <a:ln w="9525">
                 <a:solidFill>
                   <a:schemeClr val="accent3"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:errBars>
-            <c:errDir val="x"/>
-            <c:errBarType val="both"/>
-            <c:errValType val="cust"/>
-            <c:noEndCap val="0"/>
-            <c:plus>
-              <c:numRef>
-                <c:f>NE_Pipe_and_Samples!$H$4</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="1"/>
-                  <c:pt idx="0">
-                    <c:v>2E-3</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:plus>
-            <c:minus>
-              <c:numRef>
-                <c:f>NE_Pipe_and_Samples!$H$4</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="1"/>
-                  <c:pt idx="0">
-                    <c:v>2E-3</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:minus>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:errBars>
-          <c:errBars>
-            <c:errDir val="y"/>
-            <c:errBarType val="both"/>
-            <c:errValType val="cust"/>
-            <c:noEndCap val="0"/>
-            <c:plus>
-              <c:numRef>
-                <c:f>NE_Pipe_and_Samples!$J$4</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="1"/>
-                  <c:pt idx="0">
-                    <c:v>5.0000000000000001E-3</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:plus>
-            <c:minus>
-              <c:numRef>
-                <c:f>NE_Pipe_and_Samples!$J$4</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="1"/>
-                  <c:pt idx="0">
-                    <c:v>5.0000000000000001E-3</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:minus>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:errBars>
-          <c:xVal>
-            <c:numRef>
-              <c:f>NE_Pipe_and_Samples!$G$4</c:f>
-              <c:numCache>
-                <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>1.1850000000000001</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>NE_Pipe_and_Samples!$I$4</c:f>
-              <c:numCache>
-                <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>2.4660000000000002</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-1B36-4D49-962A-284DCF0BF1F4}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>NE_Pipe_and_Samples!$B$5</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Geological</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent4"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:errBars>
-            <c:errDir val="x"/>
-            <c:errBarType val="both"/>
-            <c:errValType val="cust"/>
-            <c:noEndCap val="0"/>
-            <c:plus>
-              <c:numRef>
-                <c:f>NE_Pipe_and_Samples!$H$5</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="1"/>
-                  <c:pt idx="0">
-                    <c:v>3.0000000000000001E-3</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:plus>
-            <c:minus>
-              <c:numRef>
-                <c:f>NE_Pipe_and_Samples!$H$5</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="1"/>
-                  <c:pt idx="0">
-                    <c:v>3.0000000000000001E-3</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:minus>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:errBars>
-          <c:errBars>
-            <c:errDir val="y"/>
-            <c:errBarType val="both"/>
-            <c:errValType val="cust"/>
-            <c:noEndCap val="0"/>
-            <c:plus>
-              <c:numRef>
-                <c:f>NE_Pipe_and_Samples!$J$5</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="1"/>
-                  <c:pt idx="0">
-                    <c:v>1.4999999999999999E-2</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:plus>
-            <c:minus>
-              <c:numRef>
-                <c:f>NE_Pipe_and_Samples!$J$5</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="1"/>
-                  <c:pt idx="0">
-                    <c:v>1.4999999999999999E-2</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:minus>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:errBars>
-          <c:xVal>
-            <c:numRef>
-              <c:f>NE_Pipe_and_Samples!$G$5</c:f>
-              <c:numCache>
-                <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>1.218</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>NE_Pipe_and_Samples!$I$5</c:f>
-              <c:numCache>
-                <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>2.4649999999999999</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-1B36-4D49-962A-284DCF0BF1F4}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>NE_Pipe_and_Samples!$B$6</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Geological</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent5"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -996,7 +718,7 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1.147</c:v>
+                  <c:v>1.1850000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1004,6 +726,312 @@
           <c:yVal>
             <c:numRef>
               <c:f>NE_Pipe_and_Samples!$I$6</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2.4660000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-1B36-4D49-962A-284DCF0BF1F4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>NE_Pipe_and_Samples!$B$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Geological (river)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:errBars>
+            <c:errDir val="x"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>NE_Pipe_and_Samples!$H$7</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="1"/>
+                  <c:pt idx="0">
+                    <c:v>3.0000000000000001E-3</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>NE_Pipe_and_Samples!$H$7</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="1"/>
+                  <c:pt idx="0">
+                    <c:v>3.0000000000000001E-3</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>NE_Pipe_and_Samples!$J$7</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="1"/>
+                  <c:pt idx="0">
+                    <c:v>1.4999999999999999E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>NE_Pipe_and_Samples!$J$7</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="1"/>
+                  <c:pt idx="0">
+                    <c:v>1.4999999999999999E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:xVal>
+            <c:numRef>
+              <c:f>NE_Pipe_and_Samples!$G$7</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1.218</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>NE_Pipe_and_Samples!$I$7</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2.4649999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-1B36-4D49-962A-284DCF0BF1F4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>NE_Pipe_and_Samples!$B$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Geological (lake)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:errBars>
+            <c:errDir val="x"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>NE_Pipe_and_Samples!$H$8</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="1"/>
+                  <c:pt idx="0">
+                    <c:v>2E-3</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>NE_Pipe_and_Samples!$H$8</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="1"/>
+                  <c:pt idx="0">
+                    <c:v>2E-3</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>NE_Pipe_and_Samples!$J$8</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="1"/>
+                  <c:pt idx="0">
+                    <c:v>5.0000000000000001E-3</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>NE_Pipe_and_Samples!$J$8</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="1"/>
+                  <c:pt idx="0">
+                    <c:v>5.0000000000000001E-3</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:xVal>
+            <c:numRef>
+              <c:f>NE_Pipe_and_Samples!$G$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1.147</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>NE_Pipe_and_Samples!$I$8</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="1"/>
@@ -1025,11 +1053,11 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>NE_Pipe_and_Samples!$B$7</c:f>
+              <c:f>NE_Pipe_and_Samples!$B$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Geological</c:v>
+                  <c:v>Geological (peat) </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1063,7 +1091,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>NE_Pipe_and_Samples!$H$7</c:f>
+                <c:f>NE_Pipe_and_Samples!$H$9</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="1"/>
@@ -1075,326 +1103,12 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>NE_Pipe_and_Samples!$H$7</c:f>
+                <c:f>NE_Pipe_and_Samples!$H$9</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="1"/>
                   <c:pt idx="0">
                     <c:v>4.0000000000000001E-3</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:minus>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:errBars>
-          <c:errBars>
-            <c:errDir val="y"/>
-            <c:errBarType val="both"/>
-            <c:errValType val="cust"/>
-            <c:noEndCap val="0"/>
-            <c:plus>
-              <c:numRef>
-                <c:f>NE_Pipe_and_Samples!$J$7</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="1"/>
-                  <c:pt idx="0">
-                    <c:v>3.0000000000000001E-3</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:plus>
-            <c:minus>
-              <c:numRef>
-                <c:f>NE_Pipe_and_Samples!$J$7</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="1"/>
-                  <c:pt idx="0">
-                    <c:v>3.0000000000000001E-3</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:minus>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:errBars>
-          <c:xVal>
-            <c:numRef>
-              <c:f>NE_Pipe_and_Samples!$G$7</c:f>
-              <c:numCache>
-                <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>1.169</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>NE_Pipe_and_Samples!$I$7</c:f>
-              <c:numCache>
-                <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>2.4500000000000002</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000006-1B36-4D49-962A-284DCF0BF1F4}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="6"/>
-          <c:order val="6"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>NE_Pipe_and_Samples!$B$8</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>UK petrol</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1">
-                    <a:lumMod val="60000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:errBars>
-            <c:errDir val="x"/>
-            <c:errBarType val="both"/>
-            <c:errValType val="cust"/>
-            <c:noEndCap val="0"/>
-            <c:plus>
-              <c:numRef>
-                <c:f>NE_Pipe_and_Samples!$H$8</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="1"/>
-                  <c:pt idx="0">
-                    <c:v>2.4E-2</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:plus>
-            <c:minus>
-              <c:numRef>
-                <c:f>NE_Pipe_and_Samples!$H$8</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="1"/>
-                  <c:pt idx="0">
-                    <c:v>2.4E-2</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:minus>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:errBars>
-          <c:errBars>
-            <c:errDir val="y"/>
-            <c:errBarType val="both"/>
-            <c:errValType val="cust"/>
-            <c:noEndCap val="0"/>
-            <c:plus>
-              <c:numRef>
-                <c:f>NE_Pipe_and_Samples!$J$8</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="1"/>
-                  <c:pt idx="0">
-                    <c:v>1.7999999999999999E-2</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:plus>
-            <c:minus>
-              <c:numRef>
-                <c:f>NE_Pipe_and_Samples!$J$8</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="1"/>
-                  <c:pt idx="0">
-                    <c:v>1.7999999999999999E-2</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:minus>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:errBars>
-          <c:xVal>
-            <c:numRef>
-              <c:f>NE_Pipe_and_Samples!$G$8</c:f>
-              <c:numCache>
-                <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>1.0820000000000001</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>NE_Pipe_and_Samples!$I$8</c:f>
-              <c:numCache>
-                <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>2.3420000000000001</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000007-1B36-4D49-962A-284DCF0BF1F4}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="7"/>
-          <c:order val="7"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>NE_Pipe_and_Samples!$B$9</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Scottish ore </c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2">
-                    <a:lumMod val="60000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:errBars>
-            <c:errDir val="x"/>
-            <c:errBarType val="both"/>
-            <c:errValType val="cust"/>
-            <c:noEndCap val="0"/>
-            <c:plus>
-              <c:numRef>
-                <c:f>NE_Pipe_and_Samples!$H$9</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="1"/>
-                  <c:pt idx="0">
-                    <c:v>3.0000000000000001E-3</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:plus>
-            <c:minus>
-              <c:numRef>
-                <c:f>NE_Pipe_and_Samples!$H$9</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="1"/>
-                  <c:pt idx="0">
-                    <c:v>3.0000000000000001E-3</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1463,7 +1177,7 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1.17</c:v>
+                  <c:v>1.169</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1471,6 +1185,320 @@
           <c:yVal>
             <c:numRef>
               <c:f>NE_Pipe_and_Samples!$I$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2.4500000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-1B36-4D49-962A-284DCF0BF1F4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>NE_Pipe_and_Samples!$B$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>UK petrol</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:errBars>
+            <c:errDir val="x"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>NE_Pipe_and_Samples!$H$10</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="1"/>
+                  <c:pt idx="0">
+                    <c:v>2.4E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>NE_Pipe_and_Samples!$H$10</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="1"/>
+                  <c:pt idx="0">
+                    <c:v>2.4E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>NE_Pipe_and_Samples!$J$10</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="1"/>
+                  <c:pt idx="0">
+                    <c:v>1.7999999999999999E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>NE_Pipe_and_Samples!$J$10</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="1"/>
+                  <c:pt idx="0">
+                    <c:v>1.7999999999999999E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:xVal>
+            <c:numRef>
+              <c:f>NE_Pipe_and_Samples!$G$10</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1.0820000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>NE_Pipe_and_Samples!$I$10</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2.3420000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-1B36-4D49-962A-284DCF0BF1F4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>NE_Pipe_and_Samples!$B$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Scottish ore </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:errBars>
+            <c:errDir val="x"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>NE_Pipe_and_Samples!$H$11</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="1"/>
+                  <c:pt idx="0">
+                    <c:v>3.0000000000000001E-3</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>NE_Pipe_and_Samples!$H$11</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="1"/>
+                  <c:pt idx="0">
+                    <c:v>3.0000000000000001E-3</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>NE_Pipe_and_Samples!$J$11</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="1"/>
+                  <c:pt idx="0">
+                    <c:v>3.0000000000000001E-3</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>NE_Pipe_and_Samples!$J$11</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="1"/>
+                  <c:pt idx="0">
+                    <c:v>3.0000000000000001E-3</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:xVal>
+            <c:numRef>
+              <c:f>NE_Pipe_and_Samples!$G$11</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1.17</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>NE_Pipe_and_Samples!$I$11</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="1"/>
@@ -1492,11 +1520,11 @@
           <c:order val="8"/>
           <c:tx>
             <c:strRef>
-              <c:f>NE_Pipe_and_Samples!$B$10</c:f>
+              <c:f>NE_Pipe_and_Samples!$B$12</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Water sample</c:v>
+                  <c:v>NJ Water sample</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1513,14 +1541,17 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent3">
-                  <a:lumMod val="60000"/>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="40000"/>
+                  <a:lumOff val="60000"/>
+                  <a:alpha val="20000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent3">
-                    <a:lumMod val="60000"/>
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="40000"/>
+                    <a:lumOff val="60000"/>
                   </a:schemeClr>
                 </a:solidFill>
               </a:ln>
@@ -1529,7 +1560,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>NE_Pipe_and_Samples!$G$10:$G$30</c:f>
+              <c:f>NE_Pipe_and_Samples!$G$12:$G$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
@@ -1601,7 +1632,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>NE_Pipe_and_Samples!$I$10:$I$30</c:f>
+              <c:f>NE_Pipe_and_Samples!$I$12:$I$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
@@ -1675,6 +1706,320 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000000A-1B36-4D49-962A-284DCF0BF1F4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>NE_Pipe_and_Samples!$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Edi/EL pipe</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:errBars>
+            <c:errDir val="x"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>NE_Pipe_and_Samples!$H$2</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="1"/>
+                  <c:pt idx="0">
+                    <c:v>2E-3</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>NE_Pipe_and_Samples!$H$2</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="1"/>
+                  <c:pt idx="0">
+                    <c:v>2E-3</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>NE_Pipe_and_Samples!$J$2</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="1"/>
+                  <c:pt idx="0">
+                    <c:v>2E-3</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>NE_Pipe_and_Samples!$J$2</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="1"/>
+                  <c:pt idx="0">
+                    <c:v>2E-3</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:xVal>
+            <c:numRef>
+              <c:f>NE_Pipe_and_Samples!$G$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1.17</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>NE_Pipe_and_Samples!$I$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2.4510000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-5453-4B12-9BEC-B2BEED6CAC4E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="10"/>
+          <c:order val="10"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>NE_Pipe_and_Samples!$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>G pipe</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:errBars>
+            <c:errDir val="x"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>NE_Pipe_and_Samples!$H$3</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="1"/>
+                  <c:pt idx="0">
+                    <c:v>5.0000000000000001E-3</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>NE_Pipe_and_Samples!$H$3</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="1"/>
+                  <c:pt idx="0">
+                    <c:v>5.0000000000000001E-3</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>NE_Pipe_and_Samples!$J$3</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="1"/>
+                  <c:pt idx="0">
+                    <c:v>6.0000000000000001E-3</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>NE_Pipe_and_Samples!$J$3</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="1"/>
+                  <c:pt idx="0">
+                    <c:v>6.0000000000000001E-3</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:xVal>
+            <c:numRef>
+              <c:f>NE_Pipe_and_Samples!$G$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1.17</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>NE_Pipe_and_Samples!$I$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2.4390000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-5453-4B12-9BEC-B2BEED6CAC4E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1693,6 +2038,7 @@
         <c:axId val="733818760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="1.1500000000000001"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1755,7 +2101,7 @@
         <c:axId val="733815560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="2.2999999999999998"/>
+          <c:min val="2.42"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1824,6 +2170,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.79914446864354727"/>
+          <c:y val="8.2904562474871116E-2"/>
+          <c:w val="0.20085553135645279"/>
+          <c:h val="0.84327662016005223"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2457,16 +2813,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>90487</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>180974</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>166687</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>228599</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2791,16 +3147,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DD4DC9E-06CF-4DA3-831B-C00651BC599B}">
-  <dimension ref="A1:J30"/>
+  <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="B7" sqref="B7:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.140625" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="4" width="18.140625" customWidth="1"/>
     <col min="5" max="5" width="25" customWidth="1"/>
@@ -2832,95 +3188,96 @@
         <v>17</v>
       </c>
       <c r="H1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I1" t="s">
         <v>18</v>
       </c>
       <c r="J1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G2" s="1">
-        <v>1.1326363249560998</v>
+        <v>44</v>
+      </c>
+      <c r="G2">
+        <v>1.17</v>
       </c>
       <c r="H2">
-        <v>6.0000000000000001E-3</v>
-      </c>
-      <c r="I2" s="1">
-        <v>2.4255835968166899</v>
+        <v>2E-3</v>
+      </c>
+      <c r="I2">
+        <v>2.4510000000000001</v>
       </c>
       <c r="J2">
-        <v>6.0000000000000001E-3</v>
+        <v>2E-3</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>38</v>
-      </c>
-      <c r="G3" s="2">
-        <v>1.117</v>
+        <v>45</v>
+      </c>
+      <c r="G3">
+        <v>1.17</v>
       </c>
       <c r="H3">
-        <v>0.03</v>
-      </c>
-      <c r="I3" s="2">
-        <v>2.4220000000000002</v>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="I3">
+        <v>2.4390000000000001</v>
       </c>
       <c r="J3">
-        <v>6.2E-2</v>
+        <v>6.0000000000000001E-3</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G4" s="2">
-        <v>1.1850000000000001</v>
+        <v>37</v>
+      </c>
+      <c r="G4" s="1">
+        <v>1.133</v>
       </c>
       <c r="H4">
-        <v>2E-3</v>
-      </c>
-      <c r="I4" s="2">
-        <v>2.4660000000000002</v>
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="I4" s="1">
+        <f>2.42558359681669 + 0.01</f>
+        <v>2.4355835968166897</v>
       </c>
       <c r="J4">
-        <v>5.0000000000000001E-3</v>
+        <v>6.0000000000000001E-3</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G5" s="2">
-        <v>1.218</v>
+        <v>1.117</v>
       </c>
       <c r="H5">
-        <v>3.0000000000000001E-3</v>
+        <v>0.03</v>
       </c>
       <c r="I5" s="2">
-        <v>2.4649999999999999</v>
+        <v>2.4220000000000002</v>
       </c>
       <c r="J5">
-        <v>1.4999999999999999E-2</v>
+        <v>6.2E-2</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G6" s="2">
-        <v>1.147</v>
+        <v>1.1850000000000001</v>
       </c>
       <c r="H6">
         <v>2E-3</v>
       </c>
       <c r="I6" s="2">
-        <v>2.4279999999999999</v>
+        <v>2.4660000000000002</v>
       </c>
       <c r="J6">
         <v>5.0000000000000001E-3</v>
@@ -2928,113 +3285,95 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="G7" s="2">
-        <v>1.169</v>
+        <v>1.218</v>
       </c>
       <c r="H7">
-        <v>4.0000000000000001E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="I7" s="2">
-        <v>2.4500000000000002</v>
+        <v>2.4649999999999999</v>
       </c>
       <c r="J7">
-        <v>3.0000000000000001E-3</v>
+        <v>1.4999999999999999E-2</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="G8" s="2">
-        <v>1.0820000000000001</v>
+        <v>1.147</v>
       </c>
       <c r="H8">
-        <v>2.4E-2</v>
+        <v>2E-3</v>
       </c>
       <c r="I8" s="2">
-        <v>2.3420000000000001</v>
+        <v>2.4279999999999999</v>
       </c>
       <c r="J8">
-        <v>1.7999999999999999E-2</v>
+        <v>5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>42</v>
-      </c>
-      <c r="G9" s="1">
-        <v>1.17</v>
+        <v>49</v>
+      </c>
+      <c r="G9" s="2">
+        <v>1.169</v>
       </c>
       <c r="H9">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="I9" s="1">
-        <v>2.44</v>
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="I9" s="2">
+        <v>2.4500000000000002</v>
       </c>
       <c r="J9">
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>20</v>
-      </c>
       <c r="B10" t="s">
-        <v>45</v>
-      </c>
-      <c r="C10" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" t="s">
-        <v>2</v>
-      </c>
-      <c r="E10" t="s">
-        <v>3</v>
-      </c>
-      <c r="F10">
-        <v>34.950000000000003</v>
-      </c>
-      <c r="G10">
-        <v>1.1579999999999999</v>
-      </c>
-      <c r="I10">
-        <v>2.4860000000000002</v>
+        <v>40</v>
+      </c>
+      <c r="G10" s="2">
+        <v>1.0820000000000001</v>
+      </c>
+      <c r="H10">
+        <v>2.4E-2</v>
+      </c>
+      <c r="I10" s="2">
+        <v>2.3420000000000001</v>
+      </c>
+      <c r="J10">
+        <v>1.7999999999999999E-2</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>22</v>
-      </c>
       <c r="B11" t="s">
-        <v>45</v>
-      </c>
-      <c r="C11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" t="s">
-        <v>2</v>
-      </c>
-      <c r="E11" t="s">
-        <v>3</v>
-      </c>
-      <c r="F11">
-        <v>0.19800000000000001</v>
-      </c>
-      <c r="G11">
-        <v>1.1315</v>
-      </c>
-      <c r="I11">
-        <v>2.4169999999999998</v>
+        <v>41</v>
+      </c>
+      <c r="G11" s="1">
+        <v>1.17</v>
+      </c>
+      <c r="H11">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="I11" s="1">
+        <v>2.44</v>
+      </c>
+      <c r="J11">
+        <v>3.0000000000000001E-3</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C12" t="s">
         <v>21</v>
@@ -3046,21 +3385,21 @@
         <v>3</v>
       </c>
       <c r="F12">
-        <v>-8.5999999999999993E-2</v>
+        <v>34.950000000000003</v>
       </c>
       <c r="G12">
-        <v>1.1359999999999999</v>
+        <v>1.1579999999999999</v>
       </c>
       <c r="I12">
-        <v>2.371</v>
+        <v>2.4860000000000002</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B13" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C13" t="s">
         <v>21</v>
@@ -3072,21 +3411,21 @@
         <v>3</v>
       </c>
       <c r="F13">
-        <v>-6.2E-2</v>
+        <v>0.19800000000000001</v>
       </c>
       <c r="G13">
-        <v>1.1080000000000001</v>
+        <v>1.1315</v>
       </c>
       <c r="I13">
-        <v>2.363</v>
+        <v>2.4169999999999998</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B14" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C14" t="s">
         <v>21</v>
@@ -3098,21 +3437,21 @@
         <v>3</v>
       </c>
       <c r="F14">
-        <v>0.63600000000000001</v>
+        <v>-8.5999999999999993E-2</v>
       </c>
       <c r="G14">
-        <v>1.1519999999999999</v>
+        <v>1.1359999999999999</v>
       </c>
       <c r="I14">
-        <v>2.4220000000000002</v>
+        <v>2.371</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B15" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C15" t="s">
         <v>21</v>
@@ -3124,24 +3463,24 @@
         <v>3</v>
       </c>
       <c r="F15">
-        <v>2.2690000000000001</v>
+        <v>-6.2E-2</v>
       </c>
       <c r="G15">
-        <v>1.1559999999999999</v>
+        <v>1.1080000000000001</v>
       </c>
       <c r="I15">
-        <v>2.0990000000000002</v>
+        <v>2.363</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B16" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C16" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="D16" t="s">
         <v>2</v>
@@ -3150,24 +3489,24 @@
         <v>3</v>
       </c>
       <c r="F16">
-        <v>0.11</v>
+        <v>0.63600000000000001</v>
       </c>
       <c r="G16">
-        <v>1.1479999999999999</v>
+        <v>1.1519999999999999</v>
       </c>
       <c r="I16">
-        <v>2.431</v>
+        <v>2.4220000000000002</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B17" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C17" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="D17" t="s">
         <v>2</v>
@@ -3176,21 +3515,21 @@
         <v>3</v>
       </c>
       <c r="F17">
-        <v>0.47199999999999998</v>
+        <v>2.2690000000000001</v>
       </c>
       <c r="G17">
-        <v>1.143</v>
+        <v>1.1559999999999999</v>
       </c>
       <c r="I17">
-        <v>2.4209999999999998</v>
+        <v>2.0990000000000002</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B18" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C18" t="s">
         <v>7</v>
@@ -3202,24 +3541,24 @@
         <v>3</v>
       </c>
       <c r="F18">
-        <v>0.53200000000000003</v>
+        <v>0.11</v>
       </c>
       <c r="G18">
-        <v>1.1180000000000001</v>
+        <v>1.1479999999999999</v>
       </c>
       <c r="I18">
-        <v>2.4</v>
+        <v>2.431</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B19" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C19" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D19" t="s">
         <v>2</v>
@@ -3228,24 +3567,24 @@
         <v>3</v>
       </c>
       <c r="F19">
-        <v>0.19800000000000001</v>
+        <v>0.47199999999999998</v>
       </c>
       <c r="G19">
-        <v>1.1459999999999999</v>
+        <v>1.143</v>
       </c>
       <c r="I19">
-        <v>2.4350000000000001</v>
+        <v>2.4209999999999998</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B20" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C20" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D20" t="s">
         <v>2</v>
@@ -3254,24 +3593,24 @@
         <v>3</v>
       </c>
       <c r="F20">
-        <v>1.2190000000000001</v>
+        <v>0.53200000000000003</v>
       </c>
       <c r="G20">
-        <v>1.159</v>
+        <v>1.1180000000000001</v>
       </c>
       <c r="I20">
-        <v>2.423</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B21" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C21" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D21" t="s">
         <v>2</v>
@@ -3280,24 +3619,24 @@
         <v>3</v>
       </c>
       <c r="F21">
-        <v>2.42</v>
+        <v>0.19800000000000001</v>
       </c>
       <c r="G21">
-        <v>1.1639999999999999</v>
+        <v>1.1459999999999999</v>
       </c>
       <c r="I21">
-        <v>2.4409999999999998</v>
+        <v>2.4350000000000001</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B22" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C22" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D22" t="s">
         <v>2</v>
@@ -3306,50 +3645,51 @@
         <v>3</v>
       </c>
       <c r="F22">
-        <v>22.68</v>
+        <v>1.2190000000000001</v>
       </c>
       <c r="G22">
-        <v>1.121</v>
+        <v>1.159</v>
       </c>
       <c r="I22">
-        <v>2.4710000000000001</v>
+        <v>2.423</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>34</v>
-      </c>
-      <c r="B23" t="s">
-        <v>45</v>
-      </c>
-      <c r="C23" t="s">
-        <v>35</v>
-      </c>
-      <c r="D23" t="s">
+      <c r="A23" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F23">
-        <v>5.782</v>
-      </c>
-      <c r="G23">
-        <v>1.163</v>
-      </c>
-      <c r="I23">
-        <v>2.4630000000000001</v>
+      <c r="F23" s="3">
+        <v>2.42</v>
+      </c>
+      <c r="G23" s="3">
+        <v>1.1639999999999999</v>
+      </c>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3">
+        <v>2.4409999999999998</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B24" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C24" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D24" t="s">
         <v>2</v>
@@ -3358,24 +3698,24 @@
         <v>3</v>
       </c>
       <c r="F24">
-        <v>0.34699999999999998</v>
+        <v>22.68</v>
       </c>
       <c r="G24">
-        <v>1.1399999999999999</v>
+        <v>1.121</v>
       </c>
       <c r="I24">
-        <v>2.387</v>
+        <v>2.4710000000000001</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="B25" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C25" t="s">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="D25" t="s">
         <v>2</v>
@@ -3384,24 +3724,24 @@
         <v>3</v>
       </c>
       <c r="F25">
-        <v>0.13200000000000001</v>
+        <v>5.782</v>
       </c>
       <c r="G25">
-        <v>1.0860000000000001</v>
+        <v>1.163</v>
       </c>
       <c r="I25">
-        <v>2.3439999999999999</v>
+        <v>2.4630000000000001</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>4</v>
+        <v>36</v>
       </c>
       <c r="B26" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C26" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D26" t="s">
         <v>2</v>
@@ -3410,24 +3750,24 @@
         <v>3</v>
       </c>
       <c r="F26">
-        <v>0.44</v>
+        <v>0.34699999999999998</v>
       </c>
       <c r="G26">
-        <v>1.1040000000000001</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="I26">
-        <v>2.3559999999999999</v>
+        <v>2.387</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B27" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C27" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D27" t="s">
         <v>2</v>
@@ -3436,21 +3776,21 @@
         <v>3</v>
       </c>
       <c r="F27">
-        <v>0.27600000000000002</v>
+        <v>0.13200000000000001</v>
       </c>
       <c r="G27">
-        <v>1.085</v>
+        <v>1.0860000000000001</v>
       </c>
       <c r="I27">
-        <v>2.3279999999999998</v>
+        <v>2.3439999999999999</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B28" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C28" t="s">
         <v>5</v>
@@ -3462,24 +3802,24 @@
         <v>3</v>
       </c>
       <c r="F28">
-        <v>0.32200000000000001</v>
+        <v>0.44</v>
       </c>
       <c r="G28">
-        <v>1.091</v>
+        <v>1.1040000000000001</v>
       </c>
       <c r="I28">
-        <v>2.355</v>
+        <v>2.3559999999999999</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B29" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C29" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D29" t="s">
         <v>2</v>
@@ -3488,24 +3828,24 @@
         <v>3</v>
       </c>
       <c r="F29">
-        <v>9.2999999999999999E-2</v>
+        <v>0.27600000000000002</v>
       </c>
       <c r="G29">
-        <v>1.119</v>
+        <v>1.085</v>
       </c>
       <c r="I29">
-        <v>2.387</v>
+        <v>2.3279999999999998</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B30" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C30" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D30" t="s">
         <v>2</v>
@@ -3514,12 +3854,64 @@
         <v>3</v>
       </c>
       <c r="F30">
+        <v>0.32200000000000001</v>
+      </c>
+      <c r="G30">
+        <v>1.091</v>
+      </c>
+      <c r="I30">
+        <v>2.355</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>9</v>
+      </c>
+      <c r="B31" t="s">
+        <v>46</v>
+      </c>
+      <c r="C31" t="s">
+        <v>10</v>
+      </c>
+      <c r="D31" t="s">
+        <v>2</v>
+      </c>
+      <c r="E31" t="s">
+        <v>3</v>
+      </c>
+      <c r="F31">
+        <v>9.2999999999999999E-2</v>
+      </c>
+      <c r="G31">
+        <v>1.119</v>
+      </c>
+      <c r="I31">
+        <v>2.387</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>11</v>
+      </c>
+      <c r="B32" t="s">
+        <v>46</v>
+      </c>
+      <c r="C32" t="s">
+        <v>1</v>
+      </c>
+      <c r="D32" t="s">
+        <v>2</v>
+      </c>
+      <c r="E32" t="s">
+        <v>3</v>
+      </c>
+      <c r="F32">
         <v>0.11600000000000001</v>
       </c>
-      <c r="G30">
+      <c r="G32">
         <v>1.1200000000000001</v>
       </c>
-      <c r="I30">
+      <c r="I32">
         <v>2.4020000000000001</v>
       </c>
     </row>

</xml_diff>